<commit_message>
upload of everything as backup. new is, among other things: divide_into_hexagons
</commit_message>
<xml_diff>
--- a/dossier10x10_normes.xlsx
+++ b/dossier10x10_normes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\Desktop\Uni\Masterarbeit\skin_by_mueller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8347235-DB7E-4B22-9D92-61166FECFC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52ED2EBA-CBB1-4C8B-AAB5-ACF5ED62FAFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1870" yWindow="1290" windowWidth="18800" windowHeight="12820" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10x10" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,15 @@
     <sheet name="20x20" sheetId="3" r:id="rId3"/>
     <sheet name="10x10 also vertical" sheetId="4" r:id="rId4"/>
     <sheet name="20x20 also vertical" sheetId="5" r:id="rId5"/>
+    <sheet name="hexagons_with_cuts" sheetId="6" r:id="rId6"/>
+    <sheet name="compliance" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2254" uniqueCount="1133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2777" uniqueCount="1318">
   <si>
     <t>lines</t>
   </si>
@@ -3423,6 +3425,561 @@
   </si>
   <si>
     <t>2.2469</t>
+  </si>
+  <si>
+    <t>shifted lines</t>
+  </si>
+  <si>
+    <t>n = 5</t>
+  </si>
+  <si>
+    <t>compliance</t>
+  </si>
+  <si>
+    <t>0.3675</t>
+  </si>
+  <si>
+    <t>0.4993</t>
+  </si>
+  <si>
+    <t>0.7213</t>
+  </si>
+  <si>
+    <t>0.9915</t>
+  </si>
+  <si>
+    <t>7.0628</t>
+  </si>
+  <si>
+    <t>0.1631</t>
+  </si>
+  <si>
+    <t>0.2196</t>
+  </si>
+  <si>
+    <t>0.2556</t>
+  </si>
+  <si>
+    <t>0.4401</t>
+  </si>
+  <si>
+    <t>2.7200</t>
+  </si>
+  <si>
+    <t>0.1115</t>
+  </si>
+  <si>
+    <t>0.0617</t>
+  </si>
+  <si>
+    <t>0.1286</t>
+  </si>
+  <si>
+    <t>0.1673</t>
+  </si>
+  <si>
+    <t>0.1935</t>
+  </si>
+  <si>
+    <t>0.2146</t>
+  </si>
+  <si>
+    <t>0.2351</t>
+  </si>
+  <si>
+    <t>1.0864</t>
+  </si>
+  <si>
+    <t>0.0358</t>
+  </si>
+  <si>
+    <t>0.0760</t>
+  </si>
+  <si>
+    <t>0.0903</t>
+  </si>
+  <si>
+    <t>0.1098</t>
+  </si>
+  <si>
+    <t>0.1478</t>
+  </si>
+  <si>
+    <t>0.2111</t>
+  </si>
+  <si>
+    <t>1.9311</t>
+  </si>
+  <si>
+    <t>0.0226</t>
+  </si>
+  <si>
+    <t>0.0548</t>
+  </si>
+  <si>
+    <t>0.0771</t>
+  </si>
+  <si>
+    <t>0.0938</t>
+  </si>
+  <si>
+    <t>0.1156</t>
+  </si>
+  <si>
+    <t>0.1496</t>
+  </si>
+  <si>
+    <t>0.1921</t>
+  </si>
+  <si>
+    <t>0.9743</t>
+  </si>
+  <si>
+    <t>0.0171</t>
+  </si>
+  <si>
+    <t>0.0206</t>
+  </si>
+  <si>
+    <t>0.0466</t>
+  </si>
+  <si>
+    <t>0.0663</t>
+  </si>
+  <si>
+    <t>0.0886</t>
+  </si>
+  <si>
+    <t>0.1207</t>
+  </si>
+  <si>
+    <t>0.1605</t>
+  </si>
+  <si>
+    <t>0.8991</t>
+  </si>
+  <si>
+    <t>0.0060</t>
+  </si>
+  <si>
+    <t>horizontal and vertical</t>
+  </si>
+  <si>
+    <t>0.0539</t>
+  </si>
+  <si>
+    <t>0.0820</t>
+  </si>
+  <si>
+    <t>0.0728</t>
+  </si>
+  <si>
+    <t>0.0868</t>
+  </si>
+  <si>
+    <t>0.0790</t>
+  </si>
+  <si>
+    <t>0.0781</t>
+  </si>
+  <si>
+    <t>0.0902</t>
+  </si>
+  <si>
+    <t>0.0773</t>
+  </si>
+  <si>
+    <t>0.0831</t>
+  </si>
+  <si>
+    <t>0.0762</t>
+  </si>
+  <si>
+    <t>0.0764</t>
+  </si>
+  <si>
+    <t>0.0752</t>
+  </si>
+  <si>
+    <t>only vertical</t>
+  </si>
+  <si>
+    <t>0.3198</t>
+  </si>
+  <si>
+    <t>0.3100</t>
+  </si>
+  <si>
+    <t>0.2978</t>
+  </si>
+  <si>
+    <t>0.3115</t>
+  </si>
+  <si>
+    <t>0.2998</t>
+  </si>
+  <si>
+    <t>0.3025</t>
+  </si>
+  <si>
+    <t>0.3154</t>
+  </si>
+  <si>
+    <t>0.3169</t>
+  </si>
+  <si>
+    <t>0.2714</t>
+  </si>
+  <si>
+    <t>0.3594</t>
+  </si>
+  <si>
+    <t>0.2879</t>
+  </si>
+  <si>
+    <t>0.2968</t>
+  </si>
+  <si>
+    <t>0.3076</t>
+  </si>
+  <si>
+    <t>0.3816</t>
+  </si>
+  <si>
+    <t>0.3702</t>
+  </si>
+  <si>
+    <t>0.3604</t>
+  </si>
+  <si>
+    <t>0.3681</t>
+  </si>
+  <si>
+    <t>0.3757</t>
+  </si>
+  <si>
+    <t>0.3321</t>
+  </si>
+  <si>
+    <t>0.3838</t>
+  </si>
+  <si>
+    <t>0.4302</t>
+  </si>
+  <si>
+    <t>0.3462</t>
+  </si>
+  <si>
+    <t>0.3705</t>
+  </si>
+  <si>
+    <t>0.3543</t>
+  </si>
+  <si>
+    <t>0.0559</t>
+  </si>
+  <si>
+    <t>0.0842</t>
+  </si>
+  <si>
+    <t>0.0761</t>
+  </si>
+  <si>
+    <t>0.0895</t>
+  </si>
+  <si>
+    <t>0.0836</t>
+  </si>
+  <si>
+    <t>0.0822</t>
+  </si>
+  <si>
+    <t>0.0791</t>
+  </si>
+  <si>
+    <t>0.0917</t>
+  </si>
+  <si>
+    <t>0.0811</t>
+  </si>
+  <si>
+    <t>0.0853</t>
+  </si>
+  <si>
+    <t>0.0794</t>
+  </si>
+  <si>
+    <t>0.0805</t>
+  </si>
+  <si>
+    <t>0.1445</t>
+  </si>
+  <si>
+    <t>0.0512</t>
+  </si>
+  <si>
+    <t>0.1367</t>
+  </si>
+  <si>
+    <t>0.1199</t>
+  </si>
+  <si>
+    <t>0.1324</t>
+  </si>
+  <si>
+    <t>0.1251</t>
+  </si>
+  <si>
+    <t>0.1306</t>
+  </si>
+  <si>
+    <t>0.1374</t>
+  </si>
+  <si>
+    <t>0.1260</t>
+  </si>
+  <si>
+    <t>0.1187</t>
+  </si>
+  <si>
+    <t>0.1532</t>
+  </si>
+  <si>
+    <t>0.1227</t>
+  </si>
+  <si>
+    <t>0.1340</t>
+  </si>
+  <si>
+    <t>0.0475</t>
+  </si>
+  <si>
+    <t>0.0410</t>
+  </si>
+  <si>
+    <t>0.0479</t>
+  </si>
+  <si>
+    <t>0.0439</t>
+  </si>
+  <si>
+    <t>0.0486</t>
+  </si>
+  <si>
+    <t>0.0406</t>
+  </si>
+  <si>
+    <t>0.0552</t>
+  </si>
+  <si>
+    <t>0.0409</t>
+  </si>
+  <si>
+    <t>0.0414</t>
+  </si>
+  <si>
+    <t>0.0487</t>
+  </si>
+  <si>
+    <t>0.0372</t>
+  </si>
+  <si>
+    <t>0.0571</t>
+  </si>
+  <si>
+    <t>0.0485</t>
+  </si>
+  <si>
+    <t>0.0591</t>
+  </si>
+  <si>
+    <t>0.0551</t>
+  </si>
+  <si>
+    <t>0.0568</t>
+  </si>
+  <si>
+    <t>0.0532</t>
+  </si>
+  <si>
+    <t>0.0624</t>
+  </si>
+  <si>
+    <t>0.0547</t>
+  </si>
+  <si>
+    <t>0.0540</t>
+  </si>
+  <si>
+    <t>0.0535</t>
+  </si>
+  <si>
+    <t>0.0507</t>
+  </si>
+  <si>
+    <t>0.0531</t>
+  </si>
+  <si>
+    <t>0.0151</t>
+  </si>
+  <si>
+    <t>0.0235</t>
+  </si>
+  <si>
+    <t>0.0209</t>
+  </si>
+  <si>
+    <t>0.0251</t>
+  </si>
+  <si>
+    <t>0.0218</t>
+  </si>
+  <si>
+    <t>0.0250</t>
+  </si>
+  <si>
+    <t>0.0216</t>
+  </si>
+  <si>
+    <t>0.0260</t>
+  </si>
+  <si>
+    <t>0.0228</t>
+  </si>
+  <si>
+    <t>0.0242</t>
+  </si>
+  <si>
+    <t>0.0221</t>
+  </si>
+  <si>
+    <t>0.0200</t>
+  </si>
+  <si>
+    <t>0.1428</t>
+  </si>
+  <si>
+    <t>0.1267</t>
+  </si>
+  <si>
+    <t>0.1349</t>
+  </si>
+  <si>
+    <t>0.1311</t>
+  </si>
+  <si>
+    <t>0.1275</t>
+  </si>
+  <si>
+    <t>0.1342</t>
+  </si>
+  <si>
+    <t>0.1301</t>
+  </si>
+  <si>
+    <t>0.1121</t>
+  </si>
+  <si>
+    <t>0.1526</t>
+  </si>
+  <si>
+    <t>0.1211</t>
+  </si>
+  <si>
+    <t>0.1298</t>
+  </si>
+  <si>
+    <t>0.0469</t>
+  </si>
+  <si>
+    <t>0.0457</t>
+  </si>
+  <si>
+    <t>0.0465</t>
+  </si>
+  <si>
+    <t>0.0454</t>
+  </si>
+  <si>
+    <t>0.0383</t>
+  </si>
+  <si>
+    <t>0.0395</t>
+  </si>
+  <si>
+    <t>0.0426</t>
+  </si>
+  <si>
+    <t>0.0362</t>
+  </si>
+  <si>
+    <t>0.0558</t>
+  </si>
+  <si>
+    <t>0.0499</t>
+  </si>
+  <si>
+    <t>0.0593</t>
+  </si>
+  <si>
+    <t>0.0506</t>
+  </si>
+  <si>
+    <t>0.0529</t>
+  </si>
+  <si>
+    <t>0.0618</t>
+  </si>
+  <si>
+    <t>0.0514</t>
+  </si>
+  <si>
+    <t>0.0565</t>
+  </si>
+  <si>
+    <t>0.0519</t>
+  </si>
+  <si>
+    <t>0.0562</t>
+  </si>
+  <si>
+    <t>0.0147</t>
+  </si>
+  <si>
+    <t>0.0231</t>
+  </si>
+  <si>
+    <t>0.0202</t>
+  </si>
+  <si>
+    <t>0.0238</t>
+  </si>
+  <si>
+    <t>0.0212</t>
+  </si>
+  <si>
+    <t>0.0220</t>
+  </si>
+  <si>
+    <t>0.0254</t>
+  </si>
+  <si>
+    <t>0.0236</t>
+  </si>
+  <si>
+    <t>0.0213</t>
+  </si>
+  <si>
+    <t>0.0224</t>
+  </si>
+  <si>
+    <t>10x10</t>
+  </si>
+  <si>
+    <t>20x20</t>
+  </si>
+  <si>
+    <t>compliance in MPa (displacement = 0.5)</t>
   </si>
 </sst>
 </file>
@@ -3448,12 +4005,24 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -3483,7 +4052,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -3492,13 +4061,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -6149,13 +6720,13 @@
       <c r="H4" s="7" t="s">
         <v>341</v>
       </c>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="11"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="8"/>
       <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
@@ -6183,13 +6754,13 @@
       <c r="H5" s="7" t="s">
         <v>347</v>
       </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="11"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="8"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
@@ -6216,13 +6787,13 @@
       <c r="H6" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="11"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="8"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
@@ -6249,13 +6820,13 @@
       <c r="H7" s="7" t="s">
         <v>361</v>
       </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="11"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="8"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
@@ -6282,13 +6853,13 @@
       <c r="H8" s="7" t="s">
         <v>368</v>
       </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="11"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="8"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
@@ -6315,13 +6886,13 @@
       <c r="H9" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="11"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="8"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
@@ -6348,13 +6919,13 @@
       <c r="H10" s="7" t="s">
         <v>382</v>
       </c>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="11"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="8"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
@@ -6381,13 +6952,13 @@
       <c r="H11" s="7" t="s">
         <v>388</v>
       </c>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="11"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="8"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
@@ -6414,13 +6985,7 @@
       <c r="H12" s="7" t="s">
         <v>394</v>
       </c>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="11"/>
+      <c r="P12" s="8"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
@@ -6447,13 +7012,13 @@
       <c r="H13" s="7" t="s">
         <v>401</v>
       </c>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="11"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="8"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
@@ -6480,13 +7045,13 @@
       <c r="H14" s="7" t="s">
         <v>408</v>
       </c>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="11"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="8"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
@@ -6513,13 +7078,13 @@
       <c r="H15" s="7" t="s">
         <v>415</v>
       </c>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="11"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="8"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
@@ -6546,13 +7111,7 @@
       <c r="H16" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="11"/>
+      <c r="P16" s="8"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
@@ -6579,22 +7138,7 @@
       <c r="H17" s="7" t="s">
         <v>427</v>
       </c>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="11"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
+      <c r="P17" s="8"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
@@ -7393,10 +7937,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C0A088-C300-42BB-98A4-750202C43103}">
-  <dimension ref="A1:P49"/>
+  <dimension ref="A1:U49"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView zoomScale="58" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="S56" sqref="S56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7405,73 +7949,91 @@
     <col min="2" max="8" width="8.7265625" customWidth="1"/>
     <col min="9" max="9" width="16.81640625" customWidth="1"/>
     <col min="10" max="16" width="8.7265625" customWidth="1"/>
+    <col min="18" max="18" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="9" t="s">
         <v>701</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="P1" s="9" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="S2" t="s">
+        <v>1178</v>
+      </c>
+      <c r="U2" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>312</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" t="s">
         <v>312</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="N3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="O3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="10" t="s">
+      <c r="P3" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R3" t="s">
+        <v>312</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>1135</v>
+      </c>
+      <c r="U3" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -7520,8 +8082,14 @@
       <c r="P4" s="3" t="s">
         <v>614</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S4" t="s">
+        <v>1205</v>
+      </c>
+      <c r="U4" s="10" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -7570,8 +8138,14 @@
       <c r="P5" s="3" t="s">
         <v>621</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S5" t="s">
+        <v>1206</v>
+      </c>
+      <c r="U5" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -7620,8 +8194,14 @@
       <c r="P6" s="3" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S6" t="s">
+        <v>1207</v>
+      </c>
+      <c r="U6" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -7670,8 +8250,14 @@
       <c r="P7" s="3" t="s">
         <v>635</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S7" t="s">
+        <v>1208</v>
+      </c>
+      <c r="U7" t="s">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -7720,8 +8306,14 @@
       <c r="P8" s="3" t="s">
         <v>642</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S8" t="s">
+        <v>422</v>
+      </c>
+      <c r="U8" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -7770,8 +8362,14 @@
       <c r="P9" s="3" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S9" t="s">
+        <v>1209</v>
+      </c>
+      <c r="U9" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -7820,8 +8418,14 @@
       <c r="P10" s="3" t="s">
         <v>656</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S10" s="10" t="s">
+        <v>1210</v>
+      </c>
+      <c r="U10" t="s">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -7870,8 +8474,14 @@
       <c r="P11" s="3" t="s">
         <v>663</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S11" t="s">
+        <v>1211</v>
+      </c>
+      <c r="U11" s="11" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -7920,8 +8530,14 @@
       <c r="P12" s="2" t="s">
         <v>669</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S12" t="s">
+        <v>377</v>
+      </c>
+      <c r="U12" t="s">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
@@ -7970,8 +8586,14 @@
       <c r="P13" s="3" t="s">
         <v>676</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S13" t="s">
+        <v>200</v>
+      </c>
+      <c r="U13" t="s">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -8020,8 +8642,14 @@
       <c r="P14" s="3" t="s">
         <v>682</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S14" s="11" t="s">
+        <v>1212</v>
+      </c>
+      <c r="U14" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>315</v>
       </c>
@@ -8070,8 +8698,14 @@
       <c r="P15" s="3" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S15" t="s">
+        <v>1213</v>
+      </c>
+      <c r="U15" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>10</v>
       </c>
@@ -8120,8 +8754,14 @@
       <c r="P16" s="2" t="s">
         <v>694</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S16" t="s">
+        <v>1214</v>
+      </c>
+      <c r="U16" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>11</v>
       </c>
@@ -8170,76 +8810,89 @@
       <c r="P17" s="2" t="s">
         <v>700</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A19" s="9" t="s">
+      <c r="S17" t="s">
+        <v>1215</v>
+      </c>
+      <c r="U17" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>313</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I19" s="9" t="s">
+      <c r="I19" t="s">
         <v>313</v>
       </c>
-      <c r="J19" s="10" t="s">
+      <c r="J19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K19" s="10" t="s">
+      <c r="K19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L19" s="10" t="s">
+      <c r="L19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M19" s="10" t="s">
+      <c r="M19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N19" s="10" t="s">
+      <c r="N19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O19" s="10" t="s">
+      <c r="O19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="P19" s="10" t="s">
+      <c r="P19" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R19" t="s">
+        <v>313</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>1135</v>
+      </c>
+      <c r="U19" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>0</v>
       </c>
@@ -8288,8 +8941,14 @@
       <c r="P20" s="3" t="s">
         <v>708</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S20" t="s">
+        <v>1228</v>
+      </c>
+      <c r="U20" s="10" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>1</v>
       </c>
@@ -8338,8 +8997,14 @@
       <c r="P21" s="3" t="s">
         <v>714</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S21" t="s">
+        <v>1230</v>
+      </c>
+      <c r="U21" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>2</v>
       </c>
@@ -8388,8 +9053,14 @@
       <c r="P22" s="3" t="s">
         <v>721</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S22" t="s">
+        <v>1231</v>
+      </c>
+      <c r="U22" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
@@ -8438,8 +9109,14 @@
       <c r="P23" s="3" t="s">
         <v>727</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S23" t="s">
+        <v>1232</v>
+      </c>
+      <c r="U23" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>4</v>
       </c>
@@ -8488,8 +9165,14 @@
       <c r="P24" s="3" t="s">
         <v>732</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S24" t="s">
+        <v>1233</v>
+      </c>
+      <c r="U24" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>5</v>
       </c>
@@ -8538,8 +9221,14 @@
       <c r="P25" s="3" t="s">
         <v>739</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S25" t="s">
+        <v>244</v>
+      </c>
+      <c r="U25" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>6</v>
       </c>
@@ -8588,8 +9277,14 @@
       <c r="P26" s="3" t="s">
         <v>745</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S26" t="s">
+        <v>1234</v>
+      </c>
+      <c r="U26" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>7</v>
       </c>
@@ -8638,8 +9333,14 @@
       <c r="P27" s="3" t="s">
         <v>751</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S27" t="s">
+        <v>1235</v>
+      </c>
+      <c r="U27" s="11" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>8</v>
       </c>
@@ -8688,8 +9389,14 @@
       <c r="P28" s="2" t="s">
         <v>755</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S28" t="s">
+        <v>1236</v>
+      </c>
+      <c r="U28" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>9</v>
       </c>
@@ -8738,8 +9445,14 @@
       <c r="P29" s="3" t="s">
         <v>760</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S29" s="10" t="s">
+        <v>1237</v>
+      </c>
+      <c r="U29" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
@@ -8788,8 +9501,14 @@
       <c r="P30" s="2" t="s">
         <v>765</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S30" s="11" t="s">
+        <v>1238</v>
+      </c>
+      <c r="U30" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
         <v>315</v>
       </c>
@@ -8838,8 +9557,14 @@
       <c r="P31" s="2" t="s">
         <v>772</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S31" t="s">
+        <v>609</v>
+      </c>
+      <c r="U31" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>10</v>
       </c>
@@ -8888,8 +9613,14 @@
       <c r="P32" s="2" t="s">
         <v>779</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S32" t="s">
+        <v>1239</v>
+      </c>
+      <c r="U32" t="s">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>11</v>
       </c>
@@ -8938,76 +9669,89 @@
       <c r="P33" s="3" t="s">
         <v>785</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A34" s="9"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="10"/>
-      <c r="M34" s="10"/>
-      <c r="N34" s="10"/>
-      <c r="O34" s="10"/>
-      <c r="P34" s="10"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A35" s="9" t="s">
+      <c r="S33" t="s">
+        <v>1240</v>
+      </c>
+      <c r="U33" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>314</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D35" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E35" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F35" s="10" t="s">
+      <c r="F35" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G35" s="10" t="s">
+      <c r="G35" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H35" s="10" t="s">
+      <c r="H35" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I35" s="9" t="s">
+      <c r="I35" t="s">
         <v>314</v>
       </c>
-      <c r="J35" s="10" t="s">
+      <c r="J35" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K35" s="10" t="s">
+      <c r="K35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L35" s="10" t="s">
+      <c r="L35" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M35" s="10" t="s">
+      <c r="M35" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N35" s="10" t="s">
+      <c r="N35" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O35" s="10" t="s">
+      <c r="O35" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="P35" s="10" t="s">
+      <c r="P35" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R35" t="s">
+        <v>314</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>1135</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>0</v>
       </c>
@@ -9056,8 +9800,14 @@
       <c r="P36" s="7" t="s">
         <v>789</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S36" t="s">
+        <v>1229</v>
+      </c>
+      <c r="U36" s="10" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>1</v>
       </c>
@@ -9106,8 +9856,14 @@
       <c r="P37" s="7" t="s">
         <v>796</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S37" t="s">
+        <v>1241</v>
+      </c>
+      <c r="U37" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>2</v>
       </c>
@@ -9156,8 +9912,14 @@
       <c r="P38" s="7" t="s">
         <v>800</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S38" t="s">
+        <v>925</v>
+      </c>
+      <c r="U38" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>3</v>
       </c>
@@ -9206,8 +9968,14 @@
       <c r="P39" s="7" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S39" t="s">
+        <v>1241</v>
+      </c>
+      <c r="U39" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>4</v>
       </c>
@@ -9256,8 +10024,14 @@
       <c r="P40" s="7" t="s">
         <v>810</v>
       </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S40" t="s">
+        <v>1242</v>
+      </c>
+      <c r="U40" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>5</v>
       </c>
@@ -9306,8 +10080,14 @@
       <c r="P41" s="7" t="s">
         <v>817</v>
       </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S41" t="s">
+        <v>1243</v>
+      </c>
+      <c r="U41" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>6</v>
       </c>
@@ -9356,8 +10136,14 @@
       <c r="P42" s="7" t="s">
         <v>823</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S42" t="s">
+        <v>1244</v>
+      </c>
+      <c r="U42" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>7</v>
       </c>
@@ -9406,8 +10192,14 @@
       <c r="P43" s="7" t="s">
         <v>828</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S43" t="s">
+        <v>1245</v>
+      </c>
+      <c r="U43" s="11" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>8</v>
       </c>
@@ -9456,8 +10248,14 @@
       <c r="P44" s="7" t="s">
         <v>835</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S44" t="s">
+        <v>811</v>
+      </c>
+      <c r="U44" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>9</v>
       </c>
@@ -9506,8 +10304,14 @@
       <c r="P45" s="7" t="s">
         <v>841</v>
       </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S45" s="10" t="s">
+        <v>1246</v>
+      </c>
+      <c r="U45" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>23</v>
       </c>
@@ -9556,8 +10360,14 @@
       <c r="P46" s="7" t="s">
         <v>848</v>
       </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S46" s="11" t="s">
+        <v>1247</v>
+      </c>
+      <c r="U46" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>315</v>
       </c>
@@ -9606,8 +10416,14 @@
       <c r="P47" s="7" t="s">
         <v>854</v>
       </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S47" t="s">
+        <v>1248</v>
+      </c>
+      <c r="U47" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>10</v>
       </c>
@@ -9656,8 +10472,14 @@
       <c r="P48" s="7" t="s">
         <v>860</v>
       </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S48" t="s">
+        <v>1249</v>
+      </c>
+      <c r="U48" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>11</v>
       </c>
@@ -9705,6 +10527,12 @@
       </c>
       <c r="P49" s="7" t="s">
         <v>867</v>
+      </c>
+      <c r="S49" t="s">
+        <v>1250</v>
+      </c>
+      <c r="U49" t="s">
+        <v>1274</v>
       </c>
     </row>
   </sheetData>
@@ -9715,10 +10543,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3F5B362-BA51-41BB-A4F1-7983F0C13F1F}">
-  <dimension ref="A1:P49"/>
+  <dimension ref="A1:U49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView zoomScale="61" workbookViewId="0">
+      <selection activeCell="O48" sqref="O48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9727,85 +10555,103 @@
     <col min="2" max="8" width="8.7265625" customWidth="1"/>
     <col min="9" max="9" width="16.81640625" customWidth="1"/>
     <col min="10" max="16" width="8.7265625" customWidth="1"/>
+    <col min="18" max="18" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9" t="s">
         <v>701</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12" t="s">
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="S2" t="s">
+        <v>1178</v>
+      </c>
+      <c r="U2" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>312</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" t="s">
         <v>312</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="N3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="O3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="10" t="s">
+      <c r="P3" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R3" t="s">
+        <v>312</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>1135</v>
+      </c>
+      <c r="U3" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -9854,8 +10700,14 @@
       <c r="P4" s="7" t="s">
         <v>1060</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S4" t="s">
+        <v>1192</v>
+      </c>
+      <c r="U4" s="10" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -9904,8 +10756,14 @@
       <c r="P5" s="7" t="s">
         <v>1067</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S5" t="s">
+        <v>1193</v>
+      </c>
+      <c r="U5" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -9954,8 +10812,14 @@
       <c r="P6" s="7" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S6" t="s">
+        <v>1194</v>
+      </c>
+      <c r="U6" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -10004,8 +10868,14 @@
       <c r="P7" s="7" t="s">
         <v>1080</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S7" t="s">
+        <v>560</v>
+      </c>
+      <c r="U7" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -10054,8 +10924,14 @@
       <c r="P8" s="7" t="s">
         <v>1086</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S8" t="s">
+        <v>1195</v>
+      </c>
+      <c r="U8" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -10104,8 +10980,14 @@
       <c r="P9" s="7" t="s">
         <v>1093</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S9" t="s">
+        <v>1196</v>
+      </c>
+      <c r="U9" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -10154,8 +11036,14 @@
       <c r="P10" s="7" t="s">
         <v>1097</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S10" t="s">
+        <v>1197</v>
+      </c>
+      <c r="U10" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -10204,8 +11092,14 @@
       <c r="P11" s="7" t="s">
         <v>1101</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S11" t="s">
+        <v>1198</v>
+      </c>
+      <c r="U11" s="11" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -10254,8 +11148,14 @@
       <c r="P12" s="7" t="s">
         <v>1106</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S12" t="s">
+        <v>1199</v>
+      </c>
+      <c r="U12" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
@@ -10304,8 +11204,14 @@
       <c r="P13" s="7" t="s">
         <v>1111</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S13" s="10" t="s">
+        <v>1200</v>
+      </c>
+      <c r="U13" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -10354,8 +11260,14 @@
       <c r="P14" s="7" t="s">
         <v>1115</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S14" s="11" t="s">
+        <v>1201</v>
+      </c>
+      <c r="U14" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>315</v>
       </c>
@@ -10404,8 +11316,14 @@
       <c r="P15" s="7" t="s">
         <v>1119</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S15" t="s">
+        <v>1202</v>
+      </c>
+      <c r="U15" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>10</v>
       </c>
@@ -10454,8 +11372,14 @@
       <c r="P16" s="7" t="s">
         <v>1126</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S16" t="s">
+        <v>1203</v>
+      </c>
+      <c r="U16" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>11</v>
       </c>
@@ -10504,76 +11428,89 @@
       <c r="P17" s="7" t="s">
         <v>1132</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A19" s="9" t="s">
+      <c r="S17" t="s">
+        <v>1204</v>
+      </c>
+      <c r="U17" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>313</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I19" s="9" t="s">
+      <c r="I19" t="s">
         <v>313</v>
       </c>
-      <c r="J19" s="10" t="s">
+      <c r="J19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K19" s="10" t="s">
+      <c r="K19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L19" s="10" t="s">
+      <c r="L19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M19" s="10" t="s">
+      <c r="M19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N19" s="10" t="s">
+      <c r="N19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O19" s="10" t="s">
+      <c r="O19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="P19" s="10" t="s">
+      <c r="P19" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R19" t="s">
+        <v>313</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>1135</v>
+      </c>
+      <c r="U19" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>0</v>
       </c>
@@ -10622,8 +11559,14 @@
       <c r="P20" s="7" t="s">
         <v>1055</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S20" t="s">
+        <v>1276</v>
+      </c>
+      <c r="U20" s="10" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>1</v>
       </c>
@@ -10672,8 +11615,14 @@
       <c r="P21" s="7" t="s">
         <v>981</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S21" t="s">
+        <v>547</v>
+      </c>
+      <c r="U21" t="s">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>2</v>
       </c>
@@ -10722,8 +11671,14 @@
       <c r="P22" s="7" t="s">
         <v>987</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S22" t="s">
+        <v>1277</v>
+      </c>
+      <c r="U22" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
@@ -10772,8 +11727,14 @@
       <c r="P23" s="7" t="s">
         <v>994</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S23" t="s">
+        <v>1278</v>
+      </c>
+      <c r="U23" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>4</v>
       </c>
@@ -10822,8 +11783,14 @@
       <c r="P24" s="7" t="s">
         <v>999</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S24" t="s">
+        <v>1279</v>
+      </c>
+      <c r="U24" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>5</v>
       </c>
@@ -10872,8 +11839,14 @@
       <c r="P25" s="7" t="s">
         <v>1003</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S25" t="s">
+        <v>1280</v>
+      </c>
+      <c r="U25" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>6</v>
       </c>
@@ -10922,8 +11895,14 @@
       <c r="P26" s="7" t="s">
         <v>1009</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S26" t="s">
+        <v>946</v>
+      </c>
+      <c r="U26" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>7</v>
       </c>
@@ -10972,8 +11951,14 @@
       <c r="P27" s="7" t="s">
         <v>1015</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S27" t="s">
+        <v>1281</v>
+      </c>
+      <c r="U27" s="11" t="s">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>8</v>
       </c>
@@ -11022,8 +12007,14 @@
       <c r="P28" s="7" t="s">
         <v>1021</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S28" t="s">
+        <v>1282</v>
+      </c>
+      <c r="U28" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>9</v>
       </c>
@@ -11072,8 +12063,14 @@
       <c r="P29" s="7" t="s">
         <v>1028</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S29" s="10" t="s">
+        <v>1283</v>
+      </c>
+      <c r="U29" t="s">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
@@ -11122,8 +12119,14 @@
       <c r="P30" s="7" t="s">
         <v>1033</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S30" s="11" t="s">
+        <v>1284</v>
+      </c>
+      <c r="U30" t="s">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
         <v>315</v>
       </c>
@@ -11172,8 +12175,14 @@
       <c r="P31" s="7" t="s">
         <v>1039</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S31" t="s">
+        <v>1165</v>
+      </c>
+      <c r="U31" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>10</v>
       </c>
@@ -11222,8 +12231,14 @@
       <c r="P32" s="7" t="s">
         <v>1042</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S32" t="s">
+        <v>1285</v>
+      </c>
+      <c r="U32" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>11</v>
       </c>
@@ -11272,76 +12287,89 @@
       <c r="P33" s="7" t="s">
         <v>1049</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A34" s="9"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="10"/>
-      <c r="M34" s="10"/>
-      <c r="N34" s="10"/>
-      <c r="O34" s="10"/>
-      <c r="P34" s="10"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A35" s="9" t="s">
+      <c r="S33" t="s">
+        <v>1286</v>
+      </c>
+      <c r="U33" t="s">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>314</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D35" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E35" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F35" s="10" t="s">
+      <c r="F35" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G35" s="10" t="s">
+      <c r="G35" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H35" s="10" t="s">
+      <c r="H35" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I35" s="9" t="s">
+      <c r="I35" t="s">
         <v>314</v>
       </c>
-      <c r="J35" s="10" t="s">
+      <c r="J35" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K35" s="10" t="s">
+      <c r="K35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L35" s="10" t="s">
+      <c r="L35" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M35" s="10" t="s">
+      <c r="M35" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N35" s="10" t="s">
+      <c r="N35" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O35" s="10" t="s">
+      <c r="O35" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="P35" s="10" t="s">
+      <c r="P35" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R35" t="s">
+        <v>314</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>1135</v>
+      </c>
+      <c r="U35" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>0</v>
       </c>
@@ -11390,8 +12418,14 @@
       <c r="P36" s="7" t="s">
         <v>892</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S36" t="s">
+        <v>1262</v>
+      </c>
+      <c r="U36" s="10" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>1</v>
       </c>
@@ -11440,8 +12474,14 @@
       <c r="P37" s="7" t="s">
         <v>899</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S37" t="s">
+        <v>1287</v>
+      </c>
+      <c r="U37" t="s">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>2</v>
       </c>
@@ -11490,8 +12530,14 @@
       <c r="P38" s="7" t="s">
         <v>905</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S38" t="s">
+        <v>956</v>
+      </c>
+      <c r="U38" t="s">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>3</v>
       </c>
@@ -11540,8 +12586,14 @@
       <c r="P39" s="7" t="s">
         <v>911</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S39" t="s">
+        <v>829</v>
+      </c>
+      <c r="U39" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>4</v>
       </c>
@@ -11590,8 +12642,14 @@
       <c r="P40" s="7" t="s">
         <v>917</v>
       </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S40" t="s">
+        <v>918</v>
+      </c>
+      <c r="U40" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>5</v>
       </c>
@@ -11640,8 +12698,14 @@
       <c r="P41" s="7" t="s">
         <v>924</v>
       </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S41" t="s">
+        <v>1288</v>
+      </c>
+      <c r="U41" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>6</v>
       </c>
@@ -11690,8 +12754,14 @@
       <c r="P42" s="7" t="s">
         <v>930</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S42" t="s">
+        <v>1288</v>
+      </c>
+      <c r="U42" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>7</v>
       </c>
@@ -11740,8 +12810,14 @@
       <c r="P43" s="7" t="s">
         <v>937</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S43" t="s">
+        <v>1289</v>
+      </c>
+      <c r="U43" s="11" t="s">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>8</v>
       </c>
@@ -11790,8 +12866,14 @@
       <c r="P44" s="7" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S44" t="s">
+        <v>1290</v>
+      </c>
+      <c r="U44" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>9</v>
       </c>
@@ -11840,8 +12922,14 @@
       <c r="P45" s="7" t="s">
         <v>948</v>
       </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S45" s="10" t="s">
+        <v>1291</v>
+      </c>
+      <c r="U45" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>23</v>
       </c>
@@ -11890,8 +12978,14 @@
       <c r="P46" s="7" t="s">
         <v>955</v>
       </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S46" s="11" t="s">
+        <v>1261</v>
+      </c>
+      <c r="U46" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>315</v>
       </c>
@@ -11940,8 +13034,14 @@
       <c r="P47" s="7" t="s">
         <v>962</v>
       </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S47" t="s">
+        <v>1292</v>
+      </c>
+      <c r="U47" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>10</v>
       </c>
@@ -11990,8 +13090,14 @@
       <c r="P48" s="7" t="s">
         <v>969</v>
       </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S48" t="s">
+        <v>1293</v>
+      </c>
+      <c r="U48" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>11</v>
       </c>
@@ -12039,9 +13145,1843 @@
       </c>
       <c r="P49" s="7" t="s">
         <v>976</v>
+      </c>
+      <c r="S49" t="s">
+        <v>818</v>
+      </c>
+      <c r="U49" t="s">
+        <v>1314</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4A0A719-92B8-463A-B8CD-D142B69836EA}">
+  <dimension ref="A1:S49"/>
+  <sheetViews>
+    <sheetView zoomScale="76" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.54296875" customWidth="1"/>
+    <col min="2" max="8" width="8.7265625" customWidth="1"/>
+    <col min="11" max="11" width="13" customWidth="1"/>
+    <col min="12" max="18" width="8.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9" t="s">
+        <v>701</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>312</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>1135</v>
+      </c>
+      <c r="K3" t="s">
+        <v>312</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>992</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>1136</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>1137</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>1138</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>1139</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>1140</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1038</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>1155</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>1156</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>1157</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>1158</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>1159</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>1104</v>
+      </c>
+      <c r="R4" s="8" t="s">
+        <v>1160</v>
+      </c>
+      <c r="S4" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>313</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>1135</v>
+      </c>
+      <c r="K6" t="s">
+        <v>313</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="R6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>834</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>1144</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>1145</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1146</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1133</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>1162</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>1163</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>1164</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>1165</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>1166</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>1167</v>
+      </c>
+      <c r="R7" s="8" t="s">
+        <v>1168</v>
+      </c>
+      <c r="S7" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="1"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>314</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>1135</v>
+      </c>
+      <c r="K9" t="s">
+        <v>314</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="P9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="R9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>1148</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>1149</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>1150</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>1151</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>1152</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>1153</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1154</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1133</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>1170</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>1171</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>1172</v>
+      </c>
+      <c r="O10" s="8" t="s">
+        <v>1173</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>1174</v>
+      </c>
+      <c r="Q10" s="8" t="s">
+        <v>1175</v>
+      </c>
+      <c r="R10" s="8" t="s">
+        <v>1176</v>
+      </c>
+      <c r="S10" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" t="s">
+        <v>1134</v>
+      </c>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A17" s="5"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="8"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="8"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="8"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="8"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A31" s="5"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="8"/>
+      <c r="R31" s="8"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
+      <c r="R32" s="8"/>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
+      <c r="Q33" s="8"/>
+      <c r="R33" s="8"/>
+    </row>
+    <row r="34" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8"/>
+      <c r="R36" s="8"/>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="8"/>
+      <c r="R37" s="8"/>
+    </row>
+    <row r="38" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="8"/>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
+    </row>
+    <row r="40" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+      <c r="R40" s="8"/>
+    </row>
+    <row r="41" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="8"/>
+      <c r="R41" s="8"/>
+    </row>
+    <row r="42" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
+      <c r="Q42" s="8"/>
+      <c r="R42" s="8"/>
+    </row>
+    <row r="43" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="8"/>
+      <c r="Q43" s="8"/>
+      <c r="R43" s="8"/>
+    </row>
+    <row r="44" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="8"/>
+      <c r="O44" s="8"/>
+      <c r="P44" s="8"/>
+      <c r="Q44" s="8"/>
+      <c r="R44" s="8"/>
+    </row>
+    <row r="45" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="8"/>
+      <c r="O45" s="8"/>
+      <c r="P45" s="8"/>
+      <c r="Q45" s="8"/>
+      <c r="R45" s="8"/>
+    </row>
+    <row r="46" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="8"/>
+      <c r="N46" s="8"/>
+      <c r="O46" s="8"/>
+      <c r="P46" s="8"/>
+      <c r="Q46" s="8"/>
+      <c r="R46" s="8"/>
+    </row>
+    <row r="47" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="L47" s="8"/>
+      <c r="M47" s="8"/>
+      <c r="N47" s="8"/>
+      <c r="O47" s="8"/>
+      <c r="P47" s="8"/>
+      <c r="Q47" s="8"/>
+      <c r="R47" s="8"/>
+    </row>
+    <row r="48" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="L48" s="8"/>
+      <c r="M48" s="8"/>
+      <c r="N48" s="8"/>
+      <c r="O48" s="8"/>
+      <c r="P48" s="8"/>
+      <c r="Q48" s="8"/>
+      <c r="R48" s="8"/>
+    </row>
+    <row r="49" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="L49" s="8"/>
+      <c r="M49" s="8"/>
+      <c r="N49" s="8"/>
+      <c r="O49" s="8"/>
+      <c r="P49" s="8"/>
+      <c r="Q49" s="8"/>
+      <c r="R49" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FA5382-404D-4BE0-BF00-299F339AFA3F}">
+  <dimension ref="A1:E50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="22.36328125" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" customWidth="1"/>
+    <col min="4" max="4" width="22.36328125" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>1315</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1191</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1178</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1205</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>1216</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>1217</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>1193</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>1194</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>1219</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>1220</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1209</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>1221</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>1196</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>1222</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>1197</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>1223</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>1198</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>1224</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>1199</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>1222</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>1200</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>1201</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>1226</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>1202</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>1203</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>1204</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>313</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>1251</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>1252</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>1277</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>1254</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>1278</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>1279</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>1256</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>1280</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>1257</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>946</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>1258</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>1281</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>1259</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>1282</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>1260</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>1283</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>1284</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>1261</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>1262</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>1285</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>1263</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>1286</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>314</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>1264</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>1262</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>1265</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>1287</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>925</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>1266</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>956</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>1267</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>829</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>1268</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>918</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>1269</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>1288</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>1288</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>1289</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>1290</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>1246</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>1291</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>1273</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>1261</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>1274</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>1292</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>1293</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>1250</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>1274</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>818</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>